<commit_message>
added iteratively lookback feature
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meilinlyu/VSCodeProjects/Comp 370/HW6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162666DF-37C5-4F4A-A03A-A07B182DADA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70DF847F-D6A7-D24F-A900-9ECBBA58A5FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11900" yWindow="760" windowWidth="34560" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2240" yWindow="760" windowWidth="34560" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3707,7 +3707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>

</xml_diff>